<commit_message>
finished training hundreds of hours
</commit_message>
<xml_diff>
--- a/Data/Modeling Stage/Feature Selection/Nova_IMS_feature_selection_Date_threshold_100_no_test.xlsx
+++ b/Data/Modeling Stage/Feature Selection/Nova_IMS_feature_selection_Date_threshold_100_no_test.xlsx
@@ -61,31 +61,40 @@
     <t>Total time online (min)</t>
   </si>
   <si>
-    <t>Days with no interaction (%)</t>
-  </si>
-  <si>
     <t>Clicks (% of course total)</t>
   </si>
   <si>
     <t>Resources viewed</t>
   </si>
   <si>
+    <t>Days with no interaction (%)</t>
+  </si>
+  <si>
     <t>Clicks on course</t>
+  </si>
+  <si>
+    <t>Links viewed</t>
+  </si>
+  <si>
+    <t>Start of Session 1 (%)</t>
   </si>
   <si>
     <t>Number of clicks</t>
   </si>
   <si>
-    <t>Links viewed</t>
+    <t>Clicks per session</t>
+  </si>
+  <si>
+    <t>Clicks per day</t>
   </si>
   <si>
     <t>Start of Session 2 (%)</t>
   </si>
   <si>
-    <t>Start of Session 1 (%)</t>
+    <t>Average session duration (min)</t>
   </si>
   <si>
-    <t>Clicks per day</t>
+    <t>Number of days</t>
   </si>
   <si>
     <t>Number of sessions</t>
@@ -94,22 +103,25 @@
     <t>Start of Session 3 (%)</t>
   </si>
   <si>
-    <t>Average session duration (min)</t>
-  </si>
-  <si>
-    <t>Clicks per session</t>
-  </si>
-  <si>
-    <t>Number of days</t>
+    <t>Files downloaded</t>
   </si>
   <si>
     <t>Assignments viewed</t>
   </si>
   <si>
-    <t>Files downloaded</t>
+    <t>Assignments submitted</t>
   </si>
   <si>
     <t>Start of Session 5 (%)</t>
+  </si>
+  <si>
+    <t>Clicks on folder</t>
+  </si>
+  <si>
+    <t>Clicks on forum</t>
+  </si>
+  <si>
+    <t>Start of Session 4 (%)</t>
   </si>
   <si>
     <t>Start of Session 10 (%)</t>
@@ -118,34 +130,22 @@
     <t>Start of Session 8 (%)</t>
   </si>
   <si>
+    <t>Start of Session 7 (%)</t>
+  </si>
+  <si>
     <t>Discussions viewed</t>
   </si>
   <si>
-    <t>Clicks on folder</t>
+    <t>Start of Session 9 (%)</t>
   </si>
   <si>
-    <t>Assignments submitted</t>
-  </si>
-  <si>
-    <t>Clicks on forum</t>
-  </si>
-  <si>
-    <t>Start of Session 7 (%)</t>
+    <t>Quizzes started</t>
   </si>
   <si>
     <t>Start of Session 6 (%)</t>
   </si>
   <si>
-    <t>Quizzes started</t>
-  </si>
-  <si>
     <t>Forum posts</t>
-  </si>
-  <si>
-    <t>Start of Session 4 (%)</t>
-  </si>
-  <si>
-    <t>Start of Session 9 (%)</t>
   </si>
   <si>
     <t>Submissions (% of course total)</t>
@@ -677,13 +677,13 @@
         <v>14</v>
       </c>
       <c r="B6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
       </c>
       <c r="D6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -741,13 +741,13 @@
         <v>16</v>
       </c>
       <c r="B8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
@@ -765,7 +765,7 @@
         <v>1</v>
       </c>
       <c r="J8">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -805,13 +805,13 @@
         <v>18</v>
       </c>
       <c r="B10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
       </c>
       <c r="D10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -869,13 +869,13 @@
         <v>20</v>
       </c>
       <c r="B12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -893,7 +893,7 @@
         <v>1</v>
       </c>
       <c r="J12">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -910,22 +910,22 @@
         <v>0</v>
       </c>
       <c r="E13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" t="b">
         <v>1</v>
       </c>
       <c r="G13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" t="b">
         <v>1</v>
       </c>
       <c r="I13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -965,7 +965,7 @@
         <v>23</v>
       </c>
       <c r="B15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" t="b">
         <v>1</v>
@@ -974,19 +974,19 @@
         <v>0</v>
       </c>
       <c r="E15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" t="b">
         <v>1</v>
       </c>
       <c r="G15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" t="b">
         <v>1</v>
       </c>
       <c r="I15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15">
         <v>5</v>
@@ -997,7 +997,7 @@
         <v>24</v>
       </c>
       <c r="B16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" t="b">
         <v>1</v>
@@ -1012,16 +1012,16 @@
         <v>1</v>
       </c>
       <c r="G16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" t="b">
         <v>1</v>
       </c>
       <c r="I16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1029,28 +1029,28 @@
         <v>25</v>
       </c>
       <c r="B17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
       </c>
       <c r="F17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" t="b">
         <v>1</v>
       </c>
       <c r="I17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17">
         <v>4</v>
@@ -1064,13 +1064,13 @@
         <v>1</v>
       </c>
       <c r="C18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
       </c>
       <c r="E18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" t="b">
         <v>1</v>
@@ -1099,13 +1099,13 @@
         <v>0</v>
       </c>
       <c r="D19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
       </c>
       <c r="F19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" t="b">
         <v>1</v>
@@ -1128,7 +1128,7 @@
         <v>0</v>
       </c>
       <c r="C20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
@@ -1149,7 +1149,7 @@
         <v>1</v>
       </c>
       <c r="J20">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1160,7 +1160,7 @@
         <v>0</v>
       </c>
       <c r="C21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" t="b">
         <v>0</v>
@@ -1181,7 +1181,7 @@
         <v>1</v>
       </c>
       <c r="J21">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1189,7 +1189,7 @@
         <v>30</v>
       </c>
       <c r="B22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" t="b">
         <v>1</v>
@@ -1204,16 +1204,16 @@
         <v>0</v>
       </c>
       <c r="G22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22" t="b">
         <v>1</v>
       </c>
       <c r="I22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1224,7 +1224,7 @@
         <v>0</v>
       </c>
       <c r="C23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" t="b">
         <v>0</v>
@@ -1245,7 +1245,7 @@
         <v>1</v>
       </c>
       <c r="J23">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1265,19 +1265,19 @@
         <v>0</v>
       </c>
       <c r="F24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" t="b">
         <v>1</v>
       </c>
       <c r="I24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1285,7 +1285,7 @@
         <v>33</v>
       </c>
       <c r="B25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" t="b">
         <v>1</v>
@@ -1300,16 +1300,16 @@
         <v>0</v>
       </c>
       <c r="G25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25" t="b">
         <v>1</v>
       </c>
       <c r="I25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1317,7 +1317,7 @@
         <v>34</v>
       </c>
       <c r="B26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" t="b">
         <v>1</v>
@@ -1329,7 +1329,7 @@
         <v>0</v>
       </c>
       <c r="F26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26" t="b">
         <v>0</v>
@@ -1349,10 +1349,10 @@
         <v>35</v>
       </c>
       <c r="B27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" t="b">
         <v>0</v>
@@ -1364,13 +1364,13 @@
         <v>0</v>
       </c>
       <c r="G27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27" t="b">
         <v>1</v>
       </c>
       <c r="I27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27">
         <v>3</v>
@@ -1381,10 +1381,10 @@
         <v>36</v>
       </c>
       <c r="B28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28" t="b">
         <v>0</v>
@@ -1396,13 +1396,13 @@
         <v>0</v>
       </c>
       <c r="G28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28" t="b">
         <v>1</v>
       </c>
       <c r="I28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28">
         <v>3</v>
@@ -1448,7 +1448,7 @@
         <v>0</v>
       </c>
       <c r="C30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
@@ -1460,16 +1460,16 @@
         <v>0</v>
       </c>
       <c r="G30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" t="b">
         <v>1</v>
       </c>
       <c r="I30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1512,7 +1512,7 @@
         <v>0</v>
       </c>
       <c r="C32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" t="b">
         <v>0</v>
@@ -1533,7 +1533,7 @@
         <v>0</v>
       </c>
       <c r="J32">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1544,7 +1544,7 @@
         <v>0</v>
       </c>
       <c r="C33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" t="b">
         <v>0</v>
@@ -1565,7 +1565,7 @@
         <v>0</v>
       </c>
       <c r="J33">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1576,7 +1576,7 @@
         <v>0</v>
       </c>
       <c r="C34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" t="b">
         <v>0</v>
@@ -1597,7 +1597,7 @@
         <v>0</v>
       </c>
       <c r="J34">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1608,7 +1608,7 @@
         <v>0</v>
       </c>
       <c r="C35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D35" t="b">
         <v>0</v>
@@ -1629,7 +1629,7 @@
         <v>0</v>
       </c>
       <c r="J35">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1679,7 +1679,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -1839,7 +1839,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -1871,7 +1871,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -1903,10 +1903,10 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="b">
         <v>1</v>
@@ -1915,7 +1915,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
@@ -1935,7 +1935,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -1967,7 +1967,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -1979,36 +1979,36 @@
         <v>0</v>
       </c>
       <c r="E11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
       </c>
       <c r="G11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" t="b">
         <v>1</v>
       </c>
       <c r="I11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" t="b">
         <v>1</v>
       </c>
       <c r="D12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" t="b">
         <v>1</v>
@@ -2031,10 +2031,10 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" t="b">
         <v>1</v>
@@ -2043,7 +2043,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
@@ -2063,7 +2063,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
@@ -2075,19 +2075,19 @@
         <v>0</v>
       </c>
       <c r="E14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="b">
         <v>1</v>
       </c>
       <c r="I14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <v>5</v>
@@ -2095,7 +2095,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
@@ -2127,13 +2127,13 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
@@ -2145,13 +2145,13 @@
         <v>1</v>
       </c>
       <c r="G16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" t="b">
         <v>1</v>
       </c>
       <c r="I16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16">
         <v>5</v>
@@ -2159,7 +2159,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -2191,7 +2191,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B18" t="b">
         <v>0</v>
@@ -2223,7 +2223,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B19" t="b">
         <v>0</v>
@@ -2255,10 +2255,10 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -2267,7 +2267,7 @@
         <v>0</v>
       </c>
       <c r="E20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
@@ -2287,10 +2287,10 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" t="b">
         <v>1</v>
@@ -2299,7 +2299,7 @@
         <v>0</v>
       </c>
       <c r="E21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" t="b">
         <v>1</v>
@@ -2319,7 +2319,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B22" t="b">
         <v>0</v>
@@ -2354,7 +2354,7 @@
         <v>34</v>
       </c>
       <c r="B23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" t="b">
         <v>1</v>
@@ -2366,16 +2366,16 @@
         <v>0</v>
       </c>
       <c r="F23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23" t="b">
         <v>1</v>
       </c>
       <c r="I23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23">
         <v>4</v>
@@ -2383,7 +2383,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B24" t="b">
         <v>0</v>
@@ -2392,36 +2392,36 @@
         <v>0</v>
       </c>
       <c r="D24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" t="b">
         <v>1</v>
       </c>
       <c r="I24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B25" t="b">
         <v>0</v>
       </c>
       <c r="C25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" t="b">
         <v>0</v>
@@ -2430,16 +2430,16 @@
         <v>0</v>
       </c>
       <c r="F25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" t="b">
         <v>1</v>
       </c>
       <c r="I25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25">
         <v>3</v>
@@ -2447,7 +2447,7 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B26" t="b">
         <v>1</v>
@@ -2479,7 +2479,7 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B27" t="b">
         <v>0</v>
@@ -2511,13 +2511,13 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" t="b">
         <v>0</v>
@@ -2543,7 +2543,7 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B29" t="b">
         <v>0</v>
@@ -2575,13 +2575,13 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B30" t="b">
         <v>0</v>
       </c>
       <c r="C30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
@@ -2602,12 +2602,12 @@
         <v>0</v>
       </c>
       <c r="J30">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B31" t="b">
         <v>0</v>
@@ -2671,7 +2671,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B33" t="b">
         <v>0</v>
@@ -2735,7 +2735,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B35" t="b">
         <v>0</v>
@@ -2812,7 +2812,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -2844,7 +2844,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -2876,7 +2876,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -2908,7 +2908,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -2940,7 +2940,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
@@ -2949,7 +2949,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -2967,15 +2967,15 @@
         <v>1</v>
       </c>
       <c r="J6">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
@@ -2987,7 +2987,7 @@
         <v>1</v>
       </c>
       <c r="F7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
@@ -3004,7 +3004,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -3036,7 +3036,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
@@ -3068,10 +3068,10 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
@@ -3080,10 +3080,10 @@
         <v>1</v>
       </c>
       <c r="E10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" t="b">
         <v>1</v>
@@ -3095,12 +3095,12 @@
         <v>1</v>
       </c>
       <c r="J10">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -3132,10 +3132,10 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" t="b">
         <v>1</v>
@@ -3144,19 +3144,19 @@
         <v>1</v>
       </c>
       <c r="E12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
       </c>
       <c r="G12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="b">
         <v>1</v>
       </c>
       <c r="I12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12">
         <v>6</v>
@@ -3164,16 +3164,16 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" t="b">
         <v>1</v>
       </c>
       <c r="D13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" t="b">
         <v>1</v>
@@ -3182,13 +3182,13 @@
         <v>1</v>
       </c>
       <c r="G13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" t="b">
         <v>1</v>
       </c>
       <c r="I13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13">
         <v>6</v>
@@ -3196,7 +3196,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
@@ -3208,19 +3208,19 @@
         <v>0</v>
       </c>
       <c r="E14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="b">
         <v>1</v>
       </c>
       <c r="I14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <v>5</v>
@@ -3228,7 +3228,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
@@ -3260,7 +3260,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B16" t="b">
         <v>1</v>
@@ -3272,19 +3272,19 @@
         <v>0</v>
       </c>
       <c r="E16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" t="b">
         <v>1</v>
       </c>
       <c r="I16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16">
         <v>5</v>
@@ -3292,7 +3292,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -3324,7 +3324,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B18" t="b">
         <v>1</v>
@@ -3356,7 +3356,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B19" t="b">
         <v>1</v>
@@ -3388,16 +3388,16 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" t="b">
         <v>1</v>
       </c>
       <c r="D20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" t="b">
         <v>0</v>
@@ -3420,16 +3420,16 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" t="b">
         <v>1</v>
       </c>
       <c r="D21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
@@ -3452,7 +3452,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B22" t="b">
         <v>1</v>
@@ -3484,7 +3484,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B23" t="b">
         <v>0</v>
@@ -3516,7 +3516,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B24" t="b">
         <v>0</v>
@@ -3548,7 +3548,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="B25" t="b">
         <v>0</v>
@@ -3580,7 +3580,7 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B26" t="b">
         <v>0</v>
@@ -3612,7 +3612,7 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B27" t="b">
         <v>0</v>
@@ -3644,7 +3644,7 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B28" t="b">
         <v>0</v>
@@ -3676,7 +3676,7 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B29" t="b">
         <v>0</v>
@@ -3708,7 +3708,7 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="B30" t="b">
         <v>0</v>
@@ -3740,7 +3740,7 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B31" t="b">
         <v>0</v>
@@ -3772,7 +3772,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B32" t="b">
         <v>0</v>
@@ -3804,7 +3804,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B33" t="b">
         <v>0</v>
@@ -3836,7 +3836,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B34" t="b">
         <v>0</v>
@@ -3868,7 +3868,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B35" t="b">
         <v>0</v>
@@ -3945,7 +3945,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -3977,7 +3977,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -4009,7 +4009,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -4041,7 +4041,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -4050,7 +4050,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -4068,21 +4068,21 @@
         <v>1</v>
       </c>
       <c r="J5">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
       </c>
       <c r="D6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -4105,7 +4105,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -4137,7 +4137,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -4169,7 +4169,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -4201,7 +4201,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -4210,22 +4210,22 @@
         <v>1</v>
       </c>
       <c r="D10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
       </c>
       <c r="G10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" t="b">
         <v>1</v>
       </c>
       <c r="I10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10">
         <v>6</v>
@@ -4233,7 +4233,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -4242,22 +4242,22 @@
         <v>1</v>
       </c>
       <c r="D11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
       </c>
       <c r="G11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" t="b">
         <v>1</v>
       </c>
       <c r="I11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11">
         <v>6</v>
@@ -4297,7 +4297,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
@@ -4329,7 +4329,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
@@ -4341,19 +4341,19 @@
         <v>0</v>
       </c>
       <c r="E14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" t="b">
         <v>1</v>
       </c>
       <c r="I14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14">
         <v>5</v>
@@ -4361,7 +4361,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
@@ -4373,19 +4373,19 @@
         <v>0</v>
       </c>
       <c r="E15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" t="b">
         <v>1</v>
       </c>
       <c r="I15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15">
         <v>5</v>
@@ -4393,7 +4393,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B16" t="b">
         <v>1</v>
@@ -4405,19 +4405,19 @@
         <v>0</v>
       </c>
       <c r="E16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" t="b">
         <v>1</v>
       </c>
       <c r="I16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16">
         <v>5</v>
@@ -4425,7 +4425,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -4437,19 +4437,19 @@
         <v>0</v>
       </c>
       <c r="E17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" t="b">
         <v>1</v>
       </c>
       <c r="I17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17">
         <v>5</v>
@@ -4457,10 +4457,10 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" t="b">
         <v>1</v>
@@ -4472,16 +4472,16 @@
         <v>0</v>
       </c>
       <c r="F18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" t="b">
         <v>1</v>
       </c>
       <c r="I18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18">
         <v>4</v>
@@ -4521,7 +4521,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B20" t="b">
         <v>0</v>
@@ -4553,7 +4553,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B21" t="b">
         <v>0</v>
@@ -4562,7 +4562,7 @@
         <v>1</v>
       </c>
       <c r="D21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
@@ -4571,36 +4571,36 @@
         <v>0</v>
       </c>
       <c r="G21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" t="b">
         <v>1</v>
       </c>
       <c r="I21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
       </c>
       <c r="F22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22" t="b">
         <v>0</v>
@@ -4617,16 +4617,16 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B23" t="b">
         <v>0</v>
       </c>
       <c r="C23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
@@ -4635,13 +4635,13 @@
         <v>0</v>
       </c>
       <c r="G23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23" t="b">
         <v>1</v>
       </c>
       <c r="I23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23">
         <v>3</v>
@@ -4649,13 +4649,13 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B24" t="b">
         <v>0</v>
       </c>
       <c r="C24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" t="b">
         <v>0</v>
@@ -4664,16 +4664,16 @@
         <v>0</v>
       </c>
       <c r="F24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" t="b">
         <v>1</v>
       </c>
       <c r="I24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24">
         <v>3</v>
@@ -4681,22 +4681,22 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" t="b">
         <v>0</v>
       </c>
       <c r="F25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" t="b">
         <v>0</v>
@@ -4713,13 +4713,13 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B26" t="b">
         <v>0</v>
       </c>
       <c r="C26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" t="b">
         <v>1</v>
@@ -4740,12 +4740,12 @@
         <v>0</v>
       </c>
       <c r="J26">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B27" t="b">
         <v>0</v>
@@ -4777,7 +4777,7 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B28" t="b">
         <v>0</v>
@@ -4809,13 +4809,13 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B29" t="b">
         <v>0</v>
       </c>
       <c r="C29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29" t="b">
         <v>0</v>
@@ -4836,18 +4836,18 @@
         <v>0</v>
       </c>
       <c r="J29">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B30" t="b">
         <v>0</v>
       </c>
       <c r="C30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
@@ -4868,12 +4868,12 @@
         <v>0</v>
       </c>
       <c r="J30">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B31" t="b">
         <v>0</v>
@@ -4905,7 +4905,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B32" t="b">
         <v>0</v>
@@ -4937,7 +4937,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B33" t="b">
         <v>0</v>
@@ -4969,7 +4969,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B34" t="b">
         <v>0</v>
@@ -5001,7 +5001,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B35" t="b">
         <v>0</v>

</xml_diff>